<commit_message>
Enhanced code to handle website responses while running login test with valid user. Modified LoginPage.java and LoginTest.java
</commit_message>
<xml_diff>
--- a/TestData/testdata.xlsx
+++ b/TestData/testdata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ASN\eclipse_workspace\automate-se\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ASN\eclipse_workspace\SE-Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6319E43C-CF79-49B6-9E34-2412408A9D69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D87003B-76F3-49BD-B322-F49575D80A96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2268" yWindow="2268" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>username</t>
   </si>
@@ -36,25 +36,13 @@
     <t>user1@test.com</t>
   </si>
   <si>
-    <t>pass123</t>
-  </si>
-  <si>
     <t>pass124</t>
   </si>
   <si>
-    <t>pass125</t>
-  </si>
-  <si>
     <t>pass126</t>
   </si>
   <si>
     <t>user2@test.com</t>
-  </si>
-  <si>
-    <t>user3@test.com</t>
-  </si>
-  <si>
-    <t>user4@test.com</t>
   </si>
   <si>
     <t>admin@yourstore.com</t>
@@ -395,7 +383,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
@@ -415,56 +403,45 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{8791EB3A-909C-4867-83E3-7168ADD08AD4}"/>
-    <hyperlink ref="A3:A5" r:id="rId2" display="user1@test.com" xr:uid="{8D680C3C-0387-4ACF-A16D-A3F872788A2F}"/>
-    <hyperlink ref="A3" r:id="rId3" xr:uid="{3C0B9BDC-D68D-40B8-9909-69839C535F06}"/>
-    <hyperlink ref="A4" r:id="rId4" xr:uid="{BB61B60E-B098-4502-A0B3-926C9BFA9F05}"/>
-    <hyperlink ref="A5" r:id="rId5" xr:uid="{D815F80A-1C08-4466-B5C2-CC1A25F2235B}"/>
+    <hyperlink ref="A4" r:id="rId1" xr:uid="{BB61B60E-B098-4502-A0B3-926C9BFA9F05}"/>
+    <hyperlink ref="A5" r:id="rId2" xr:uid="{D815F80A-1C08-4466-B5C2-CC1A25F2235B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modified code to fetch Valid & inValid credentials from same xlsx file having 2 sheets one with valid credentials and another with invalid
</commit_message>
<xml_diff>
--- a/TestData/testdata.xlsx
+++ b/TestData/testdata.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ASN\eclipse_workspace\SE-Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D87003B-76F3-49BD-B322-F49575D80A96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15BE88C3-7848-4628-974B-B98F4B76B578}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2268" yWindow="2268" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2268" yWindow="2268" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="8">
   <si>
     <t>username</t>
   </si>
@@ -383,10 +384,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -411,37 +412,115 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A4" r:id="rId1" xr:uid="{BB61B60E-B098-4502-A0B3-926C9BFA9F05}"/>
-    <hyperlink ref="A5" r:id="rId2" xr:uid="{D815F80A-1C08-4466-B5C2-CC1A25F2235B}"/>
+    <hyperlink ref="A5" r:id="rId1" xr:uid="{BB61B60E-B098-4502-A0B3-926C9BFA9F05}"/>
+    <hyperlink ref="A6" r:id="rId2" xr:uid="{D815F80A-1C08-4466-B5C2-CC1A25F2235B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC1A0268-7DA0-43E0-81AC-F931AB36D5D7}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{9DE6868B-0FE6-4AFA-A997-CEE9A3894A02}"/>
+    <hyperlink ref="A4" r:id="rId2" xr:uid="{69672640-7884-45CF-8C89-1EF361CB7090}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Cleaned Test data to have valid and invalid credentials in their respective sheets
</commit_message>
<xml_diff>
--- a/TestData/testdata.xlsx
+++ b/TestData/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ASN\eclipse_workspace\SE-Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15BE88C3-7848-4628-974B-B98F4B76B578}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{142BD01F-B269-4B2F-A3F6-565EB39DBDCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2268" yWindow="2268" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2268" yWindow="2268" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="9">
   <si>
     <t>username</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t>admin</t>
+  </si>
+  <si>
+    <t>user3@test.com</t>
   </si>
 </sst>
 </file>
@@ -384,10 +387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -425,41 +428,21 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="A5" r:id="rId1" xr:uid="{BB61B60E-B098-4502-A0B3-926C9BFA9F05}"/>
-    <hyperlink ref="A6" r:id="rId2" xr:uid="{D815F80A-1C08-4466-B5C2-CC1A25F2235B}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -467,8 +450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC1A0268-7DA0-43E0-81AC-F931AB36D5D7}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -510,16 +493,17 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1" xr:uid="{9DE6868B-0FE6-4AFA-A997-CEE9A3894A02}"/>
     <hyperlink ref="A4" r:id="rId2" xr:uid="{69672640-7884-45CF-8C89-1EF361CB7090}"/>
+    <hyperlink ref="A5" r:id="rId3" xr:uid="{3C88A4B4-328F-4300-8584-F5E8266F1FFD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>